<commit_message>
driveTim and radius build
</commit_message>
<xml_diff>
--- a/data/warnLogs_200720.xlsx
+++ b/data/warnLogs_200720.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mmainza/Desktop/projects/warn/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6046E29-3CB8-C14C-B4E2-98F8F30410A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C15E02D-6344-6544-8E49-9A389C4492F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3380" yWindow="1480" windowWidth="31700" windowHeight="19980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3360" yWindow="1140" windowWidth="31700" windowHeight="19980" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="warnLogs" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12117" uniqueCount="4593">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12318" uniqueCount="4604">
   <si>
     <t>ID</t>
   </si>
@@ -13822,6 +13822,39 @@
   </si>
   <si>
     <t>31905</t>
+  </si>
+  <si>
+    <t>YogaWorks</t>
+  </si>
+  <si>
+    <t>48-49</t>
+  </si>
+  <si>
+    <t>Transportation and Warehousing</t>
+  </si>
+  <si>
+    <t>31-33</t>
+  </si>
+  <si>
+    <t>Manufacturing</t>
+  </si>
+  <si>
+    <t>Health Care and Social Assistance</t>
+  </si>
+  <si>
+    <t>Administrative Support and Waste Management and Remediation Services</t>
+  </si>
+  <si>
+    <t>Information</t>
+  </si>
+  <si>
+    <t>Accommodation and Food Services</t>
+  </si>
+  <si>
+    <t>Solo Cup</t>
+  </si>
+  <si>
+    <t>Other Services (except Public Administration)</t>
   </si>
 </sst>
 </file>
@@ -14204,7 +14237,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H1837"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E1838" sqref="E1838"/>
     </sheetView>
   </sheetViews>
@@ -60561,8 +60594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BCCB440-58B2-CE46-A849-62F4E1985780}">
   <dimension ref="A1:D1525"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -60639,191 +60672,296 @@
       <c r="A12" t="s">
         <v>1100</v>
       </c>
+      <c r="B12" t="s">
+        <v>813</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4594</v>
+      </c>
+      <c r="D12" t="s">
+        <v>4595</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>813</v>
       </c>
+      <c r="B13" t="s">
+        <v>813</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4594</v>
+      </c>
+      <c r="D13" t="s">
+        <v>4595</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>3286</v>
       </c>
+      <c r="B14" t="s">
+        <v>813</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4594</v>
+      </c>
+      <c r="D14" t="s">
+        <v>4595</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>1167</v>
       </c>
+      <c r="B15" t="s">
+        <v>813</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4594</v>
+      </c>
+      <c r="D15" t="s">
+        <v>4595</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C16">
+        <v>71</v>
+      </c>
+      <c r="D16" t="s">
+        <v>4574</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>3926</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>3927</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>3927</v>
+      </c>
+      <c r="C18">
+        <v>51</v>
+      </c>
+      <c r="D18" t="s">
+        <v>4600</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C19">
+        <v>52</v>
+      </c>
+      <c r="D19" t="s">
+        <v>4568</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>577</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>3928</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C21">
+        <v>62</v>
+      </c>
+      <c r="D21" t="s">
+        <v>4598</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>1437</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>3929</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>1031</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C24">
+        <v>62</v>
+      </c>
+      <c r="D24" t="s">
+        <v>4598</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>3930</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C25">
+        <v>62</v>
+      </c>
+      <c r="D25" t="s">
+        <v>4598</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>3466</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>3931</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>1192</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>3932</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>1263</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>3921</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>4516</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>3933</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>3934</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>1309</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>3935</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>3936</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>3937</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C40" t="s">
+        <v>4569</v>
+      </c>
+      <c r="D40" t="s">
+        <v>4570</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>3938</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>3939</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>3940</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>3571</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>3941</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C46" t="s">
+        <v>4596</v>
+      </c>
+      <c r="D46" t="s">
+        <v>4597</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>1246</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C47">
+        <v>61</v>
+      </c>
+      <c r="D47" t="s">
+        <v>4577</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>3942</v>
+      </c>
+      <c r="C48" t="s">
+        <v>4596</v>
+      </c>
+      <c r="D48" t="s">
+        <v>4597</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>3943</v>
       </c>
+      <c r="C49" t="s">
+        <v>4596</v>
+      </c>
+      <c r="D49" t="s">
+        <v>4597</v>
+      </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
@@ -60988,11 +61126,23 @@
       <c r="A77" t="s">
         <v>1105</v>
       </c>
+      <c r="C77" t="s">
+        <v>4594</v>
+      </c>
+      <c r="D77" t="s">
+        <v>4595</v>
+      </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>1211</v>
       </c>
+      <c r="C78" t="s">
+        <v>4594</v>
+      </c>
+      <c r="D78" t="s">
+        <v>4595</v>
+      </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
@@ -61038,11 +61188,23 @@
       <c r="A87" t="s">
         <v>1448</v>
       </c>
+      <c r="C87">
+        <v>61</v>
+      </c>
+      <c r="D87" t="s">
+        <v>4577</v>
+      </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>3957</v>
       </c>
+      <c r="C88" t="s">
+        <v>4594</v>
+      </c>
+      <c r="D88" t="s">
+        <v>4595</v>
+      </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
@@ -61078,6 +61240,12 @@
       <c r="A95" t="s">
         <v>482</v>
       </c>
+      <c r="C95">
+        <v>81</v>
+      </c>
+      <c r="D95" t="s">
+        <v>4603</v>
+      </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
@@ -61521,164 +61689,194 @@
         <v>791</v>
       </c>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>1251</v>
       </c>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>3986</v>
       </c>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>1120</v>
       </c>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>1135</v>
       </c>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>1596</v>
       </c>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>3987</v>
       </c>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>1025</v>
       </c>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>1218</v>
       </c>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>4520</v>
       </c>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C172">
+        <v>62</v>
+      </c>
+      <c r="D172" t="s">
+        <v>4598</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>1599</v>
       </c>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>1452</v>
       </c>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>1187</v>
       </c>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>3988</v>
       </c>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>3989</v>
       </c>
     </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>3990</v>
       </c>
-    </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C178" t="s">
+        <v>4569</v>
+      </c>
+      <c r="D178" t="s">
+        <v>4570</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>3991</v>
       </c>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>3992</v>
       </c>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>869</v>
       </c>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>848</v>
       </c>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>3993</v>
       </c>
     </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>3994</v>
       </c>
     </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>1465</v>
       </c>
     </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>1110</v>
       </c>
     </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>3995</v>
       </c>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>3996</v>
       </c>
-    </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C189" t="s">
+        <v>4569</v>
+      </c>
+      <c r="D189" t="s">
+        <v>4570</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>3997</v>
       </c>
-    </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C190" t="s">
+        <v>4569</v>
+      </c>
+      <c r="D190" t="s">
+        <v>4570</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>121</v>
+      </c>
+      <c r="C192">
+        <v>72</v>
+      </c>
+      <c r="D192" t="s">
+        <v>4601</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.2">
@@ -62416,6 +62614,12 @@
       <c r="B248" t="s">
         <v>1115</v>
       </c>
+      <c r="C248" t="s">
+        <v>4596</v>
+      </c>
+      <c r="D248" t="s">
+        <v>4597</v>
+      </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
@@ -62424,6 +62628,12 @@
       <c r="B249" t="s">
         <v>1115</v>
       </c>
+      <c r="C249" t="s">
+        <v>4596</v>
+      </c>
+      <c r="D249" t="s">
+        <v>4597</v>
+      </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
@@ -62452,6 +62662,12 @@
       <c r="B254" t="s">
         <v>1393</v>
       </c>
+      <c r="C254" t="s">
+        <v>4569</v>
+      </c>
+      <c r="D254" t="s">
+        <v>4570</v>
+      </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
@@ -62460,6 +62676,12 @@
       <c r="B255" t="s">
         <v>1393</v>
       </c>
+      <c r="C255" t="s">
+        <v>4569</v>
+      </c>
+      <c r="D255" t="s">
+        <v>4570</v>
+      </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
@@ -62575,6 +62797,12 @@
       <c r="A278" t="s">
         <v>369</v>
       </c>
+      <c r="C278">
+        <v>62</v>
+      </c>
+      <c r="D278" t="s">
+        <v>4598</v>
+      </c>
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
@@ -62619,6 +62847,12 @@
       <c r="B285" t="s">
         <v>4575</v>
       </c>
+      <c r="C285">
+        <v>62</v>
+      </c>
+      <c r="D285" t="s">
+        <v>4598</v>
+      </c>
     </row>
     <row r="286" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
@@ -62627,6 +62861,12 @@
       <c r="B286" t="s">
         <v>4575</v>
       </c>
+      <c r="C286">
+        <v>62</v>
+      </c>
+      <c r="D286" t="s">
+        <v>4598</v>
+      </c>
     </row>
     <row r="287" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
@@ -62635,94 +62875,124 @@
       <c r="B287" t="s">
         <v>4575</v>
       </c>
+      <c r="C287">
+        <v>62</v>
+      </c>
+      <c r="D287" t="s">
+        <v>4598</v>
+      </c>
     </row>
     <row r="288" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
         <v>4019</v>
       </c>
     </row>
-    <row r="289" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
         <v>4020</v>
       </c>
     </row>
-    <row r="290" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
         <v>4021</v>
       </c>
     </row>
-    <row r="291" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="292" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
         <v>4022</v>
       </c>
     </row>
-    <row r="293" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
         <v>4023</v>
       </c>
     </row>
-    <row r="294" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
         <v>1631</v>
       </c>
       <c r="B294" t="s">
         <v>1631</v>
       </c>
-    </row>
-    <row r="295" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C294" t="s">
+        <v>4596</v>
+      </c>
+      <c r="D294" t="s">
+        <v>4597</v>
+      </c>
+    </row>
+    <row r="295" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
         <v>4524</v>
       </c>
       <c r="B295" t="s">
         <v>1631</v>
       </c>
-    </row>
-    <row r="296" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C295" t="s">
+        <v>4596</v>
+      </c>
+      <c r="D295" t="s">
+        <v>4597</v>
+      </c>
+    </row>
+    <row r="296" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
         <v>4024</v>
       </c>
     </row>
-    <row r="297" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
         <v>4025</v>
       </c>
     </row>
-    <row r="298" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
         <v>4026</v>
       </c>
     </row>
-    <row r="299" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
         <v>1375</v>
       </c>
-    </row>
-    <row r="300" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C299">
+        <v>92</v>
+      </c>
+      <c r="D299" t="s">
+        <v>4567</v>
+      </c>
+    </row>
+    <row r="300" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
         <v>4027</v>
       </c>
     </row>
-    <row r="301" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
         <v>4028</v>
       </c>
     </row>
-    <row r="302" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
         <v>1413</v>
       </c>
     </row>
-    <row r="303" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
         <v>4029</v>
       </c>
-    </row>
-    <row r="304" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C303">
+        <v>62</v>
+      </c>
+      <c r="D303" t="s">
+        <v>4598</v>
+      </c>
+    </row>
+    <row r="304" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A304" t="s">
         <v>4030</v>
       </c>
@@ -63007,6 +63277,12 @@
       <c r="A326" t="s">
         <v>1444</v>
       </c>
+      <c r="C326">
+        <v>62</v>
+      </c>
+      <c r="D326" t="s">
+        <v>4598</v>
+      </c>
     </row>
     <row r="327" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A327" t="s">
@@ -63237,6 +63513,12 @@
       <c r="A366" t="s">
         <v>1459</v>
       </c>
+      <c r="C366">
+        <v>62</v>
+      </c>
+      <c r="D366" t="s">
+        <v>4598</v>
+      </c>
     </row>
     <row r="367" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A367" t="s">
@@ -63442,6 +63724,12 @@
       <c r="A407" t="s">
         <v>913</v>
       </c>
+      <c r="C407">
+        <v>51</v>
+      </c>
+      <c r="D407" t="s">
+        <v>4600</v>
+      </c>
     </row>
     <row r="408" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A408" t="s">
@@ -63892,82 +64180,88 @@
         <v>4089</v>
       </c>
     </row>
-    <row r="481" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="481" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A481" t="s">
         <v>4090</v>
       </c>
     </row>
-    <row r="482" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="482" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A482" t="s">
         <v>1248</v>
       </c>
     </row>
-    <row r="483" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="483" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A483" t="s">
         <v>797</v>
       </c>
     </row>
-    <row r="484" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="484" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A484" t="s">
         <v>1006</v>
       </c>
     </row>
-    <row r="485" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="485" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A485" t="s">
         <v>4091</v>
       </c>
     </row>
-    <row r="486" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="486" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A486" t="s">
         <v>1366</v>
       </c>
     </row>
-    <row r="487" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="487" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A487" t="s">
         <v>4092</v>
       </c>
     </row>
-    <row r="488" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="488" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A488" t="s">
         <v>4093</v>
       </c>
     </row>
-    <row r="489" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="489" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A489" t="s">
         <v>490</v>
       </c>
     </row>
-    <row r="490" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="490" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A490" t="s">
         <v>3423</v>
       </c>
     </row>
-    <row r="491" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="491" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A491" t="s">
         <v>3395</v>
       </c>
     </row>
-    <row r="492" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="492" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A492" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="493" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C492">
+        <v>62</v>
+      </c>
+      <c r="D492" t="s">
+        <v>4598</v>
+      </c>
+    </row>
+    <row r="493" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A493" t="s">
         <v>4094</v>
       </c>
     </row>
-    <row r="494" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="494" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A494" t="s">
         <v>4095</v>
       </c>
     </row>
-    <row r="495" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="495" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A495" t="s">
         <v>1458</v>
       </c>
     </row>
-    <row r="496" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="496" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A496" t="s">
         <v>1311</v>
       </c>
@@ -64310,6 +64604,12 @@
       <c r="A559" t="s">
         <v>1297</v>
       </c>
+      <c r="C559">
+        <v>62</v>
+      </c>
+      <c r="D559" t="s">
+        <v>4598</v>
+      </c>
     </row>
     <row r="560" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A560" t="s">
@@ -64505,6 +64805,12 @@
       <c r="A598" t="s">
         <v>3523</v>
       </c>
+      <c r="C598">
+        <v>62</v>
+      </c>
+      <c r="D598" t="s">
+        <v>4598</v>
+      </c>
     </row>
     <row r="599" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A599" t="s">
@@ -64551,6 +64857,12 @@
       <c r="A606" t="s">
         <v>1451</v>
       </c>
+      <c r="C606">
+        <v>62</v>
+      </c>
+      <c r="D606" t="s">
+        <v>4598</v>
+      </c>
     </row>
     <row r="607" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A607" t="s">
@@ -64642,82 +64954,88 @@
         <v>3320</v>
       </c>
     </row>
-    <row r="625" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="625" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A625" t="s">
         <v>1275</v>
       </c>
     </row>
-    <row r="626" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="626" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A626" t="s">
         <v>921</v>
       </c>
     </row>
-    <row r="627" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="627" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A627" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="628" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="628" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A628" t="s">
         <v>4149</v>
       </c>
-    </row>
-    <row r="629" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C628">
+        <v>62</v>
+      </c>
+      <c r="D628" t="s">
+        <v>4598</v>
+      </c>
+    </row>
+    <row r="629" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A629" t="s">
         <v>4150</v>
       </c>
     </row>
-    <row r="630" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="630" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A630" t="s">
         <v>1149</v>
       </c>
     </row>
-    <row r="631" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="631" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A631" t="s">
         <v>4151</v>
       </c>
     </row>
-    <row r="632" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="632" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A632" t="s">
         <v>4152</v>
       </c>
     </row>
-    <row r="633" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="633" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A633" t="s">
         <v>1253</v>
       </c>
     </row>
-    <row r="634" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="634" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A634" t="s">
         <v>4537</v>
       </c>
     </row>
-    <row r="635" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="635" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A635" t="s">
         <v>4153</v>
       </c>
     </row>
-    <row r="636" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="636" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A636" t="s">
         <v>4154</v>
       </c>
     </row>
-    <row r="637" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="637" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A637" t="s">
         <v>4155</v>
       </c>
     </row>
-    <row r="638" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="638" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A638" t="s">
         <v>4156</v>
       </c>
     </row>
-    <row r="639" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="639" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A639" t="s">
         <v>958</v>
       </c>
     </row>
-    <row r="640" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="640" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A640" t="s">
         <v>1460</v>
       </c>
@@ -64980,82 +65298,88 @@
         <v>441</v>
       </c>
     </row>
-    <row r="689" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="689" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A689" t="s">
         <v>4179</v>
       </c>
     </row>
-    <row r="690" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="690" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A690" t="s">
         <v>4180</v>
       </c>
     </row>
-    <row r="691" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="691" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A691" t="s">
         <v>3299</v>
       </c>
     </row>
-    <row r="692" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="692" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A692" t="s">
         <v>3553</v>
       </c>
     </row>
-    <row r="693" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="693" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A693" t="s">
         <v>1331</v>
       </c>
     </row>
-    <row r="694" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="694" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A694" t="s">
         <v>3403</v>
       </c>
     </row>
-    <row r="695" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="695" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A695" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="696" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="696" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A696" t="s">
         <v>4181</v>
       </c>
     </row>
-    <row r="697" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="697" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A697" t="s">
         <v>1357</v>
       </c>
     </row>
-    <row r="698" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="698" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A698" t="s">
         <v>795</v>
       </c>
     </row>
-    <row r="699" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="699" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A699" t="s">
         <v>1157</v>
       </c>
     </row>
-    <row r="700" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="700" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A700" t="s">
         <v>1348</v>
       </c>
-    </row>
-    <row r="701" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C700">
+        <v>62</v>
+      </c>
+      <c r="D700" t="s">
+        <v>4598</v>
+      </c>
+    </row>
+    <row r="701" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A701" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="702" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="702" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A702" t="s">
         <v>3232</v>
       </c>
     </row>
-    <row r="703" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="703" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A703" t="s">
         <v>3529</v>
       </c>
     </row>
-    <row r="704" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="704" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A704" t="s">
         <v>4182</v>
       </c>
@@ -65823,6 +66147,12 @@
       <c r="A852" t="s">
         <v>239</v>
       </c>
+      <c r="C852">
+        <v>62</v>
+      </c>
+      <c r="D852" t="s">
+        <v>4598</v>
+      </c>
     </row>
     <row r="853" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A853" t="s">
@@ -66045,82 +66375,100 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="881" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="881" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A881" t="s">
         <v>4256</v>
       </c>
     </row>
-    <row r="882" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="882" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A882" t="s">
         <v>1381</v>
       </c>
-    </row>
-    <row r="883" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C882">
+        <v>62</v>
+      </c>
+      <c r="D882" t="s">
+        <v>4598</v>
+      </c>
+    </row>
+    <row r="883" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A883" t="s">
         <v>1194</v>
       </c>
-    </row>
-    <row r="884" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C883">
+        <v>62</v>
+      </c>
+      <c r="D883" t="s">
+        <v>4598</v>
+      </c>
+    </row>
+    <row r="884" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A884" t="s">
         <v>4257</v>
       </c>
     </row>
-    <row r="885" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="885" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A885" t="s">
         <v>4258</v>
       </c>
     </row>
-    <row r="886" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="886" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A886" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="887" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="887" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A887" t="s">
         <v>1306</v>
       </c>
-    </row>
-    <row r="888" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C887" t="s">
+        <v>4596</v>
+      </c>
+      <c r="D887" t="s">
+        <v>4597</v>
+      </c>
+    </row>
+    <row r="888" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A888" t="s">
         <v>4259</v>
       </c>
     </row>
-    <row r="889" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="889" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A889" t="s">
         <v>3585</v>
       </c>
     </row>
-    <row r="890" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="890" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A890" t="s">
         <v>1370</v>
       </c>
     </row>
-    <row r="891" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="891" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A891" t="s">
         <v>4260</v>
       </c>
     </row>
-    <row r="892" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="892" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A892" t="s">
         <v>3828</v>
       </c>
     </row>
-    <row r="893" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="893" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A893" t="s">
         <v>1160</v>
       </c>
     </row>
-    <row r="894" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="894" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A894" t="s">
         <v>4548</v>
       </c>
     </row>
-    <row r="895" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="895" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A895" t="s">
         <v>4261</v>
       </c>
     </row>
-    <row r="896" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="896" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A896" t="s">
         <v>3276</v>
       </c>
@@ -66463,82 +66811,88 @@
         <v>1271</v>
       </c>
     </row>
-    <row r="961" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="961" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A961" t="s">
         <v>1119</v>
       </c>
     </row>
-    <row r="962" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="962" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A962" t="s">
         <v>4283</v>
       </c>
     </row>
-    <row r="963" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="963" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A963" t="s">
         <v>1129</v>
       </c>
     </row>
-    <row r="964" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="964" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A964" t="s">
         <v>1424</v>
       </c>
     </row>
-    <row r="965" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="965" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A965" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="966" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="966" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A966" t="s">
         <v>3589</v>
       </c>
     </row>
-    <row r="967" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="967" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A967" t="s">
         <v>4284</v>
       </c>
     </row>
-    <row r="968" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="968" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A968" t="s">
         <v>4285</v>
       </c>
     </row>
-    <row r="969" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="969" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A969" t="s">
         <v>1287</v>
       </c>
     </row>
-    <row r="970" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="970" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A970" t="s">
         <v>1231</v>
       </c>
-    </row>
-    <row r="971" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C970">
+        <v>62</v>
+      </c>
+      <c r="D970" t="s">
+        <v>4598</v>
+      </c>
+    </row>
+    <row r="971" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A971" t="s">
         <v>4286</v>
       </c>
     </row>
-    <row r="972" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="972" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A972" t="s">
         <v>4287</v>
       </c>
     </row>
-    <row r="973" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="973" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A973" t="s">
         <v>4288</v>
       </c>
     </row>
-    <row r="974" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="974" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A974" t="s">
         <v>543</v>
       </c>
     </row>
-    <row r="975" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="975" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A975" t="s">
         <v>1603</v>
       </c>
     </row>
-    <row r="976" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="976" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A976" t="s">
         <v>3208</v>
       </c>
@@ -66881,82 +67235,88 @@
         <v>4315</v>
       </c>
     </row>
-    <row r="1041" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1041" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1041" t="s">
         <v>1620</v>
       </c>
     </row>
-    <row r="1042" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1042" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1042" t="s">
         <v>4316</v>
       </c>
     </row>
-    <row r="1043" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1043" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1043" t="s">
         <v>4317</v>
       </c>
     </row>
-    <row r="1044" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1044" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1044" t="s">
         <v>4318</v>
       </c>
     </row>
-    <row r="1045" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1045" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1045" t="s">
         <v>4319</v>
       </c>
     </row>
-    <row r="1046" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1046" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1046" t="s">
         <v>4320</v>
       </c>
     </row>
-    <row r="1047" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1047" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1047" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="1048" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C1047">
+        <v>62</v>
+      </c>
+      <c r="D1047" t="s">
+        <v>4598</v>
+      </c>
+    </row>
+    <row r="1048" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1048" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="1049" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1049" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1049" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="1050" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1050" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1050" t="s">
         <v>4321</v>
       </c>
     </row>
-    <row r="1051" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1051" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1051" t="s">
         <v>1272</v>
       </c>
     </row>
-    <row r="1052" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1052" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1052" t="s">
         <v>863</v>
       </c>
     </row>
-    <row r="1053" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1053" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1053" t="s">
         <v>1098</v>
       </c>
     </row>
-    <row r="1054" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1054" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1054" t="s">
         <v>4322</v>
       </c>
     </row>
-    <row r="1055" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1055" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1055" t="s">
         <v>4323</v>
       </c>
     </row>
-    <row r="1056" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1056" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1056" t="s">
         <v>957</v>
       </c>
@@ -67139,82 +67499,88 @@
         <v>4574</v>
       </c>
     </row>
-    <row r="1089" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1089" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1089" t="s">
         <v>1475</v>
       </c>
     </row>
-    <row r="1090" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1090" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1090" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="1091" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1091" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1091" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="1092" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1092" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1092" t="s">
         <v>4336</v>
       </c>
     </row>
-    <row r="1093" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1093" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1093" t="s">
         <v>4337</v>
       </c>
     </row>
-    <row r="1094" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1094" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1094" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="1095" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1095" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1095" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="1096" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1096" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1096" t="s">
         <v>4338</v>
       </c>
     </row>
-    <row r="1097" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1097" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1097" t="s">
         <v>1425</v>
       </c>
     </row>
-    <row r="1098" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1098" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1098" t="s">
         <v>1426</v>
       </c>
     </row>
-    <row r="1099" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1099" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1099" t="s">
         <v>611</v>
       </c>
     </row>
-    <row r="1100" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1100" t="s">
         <v>4339</v>
       </c>
-    </row>
-    <row r="1101" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C1100">
+        <v>62</v>
+      </c>
+      <c r="D1100" t="s">
+        <v>4598</v>
+      </c>
+    </row>
+    <row r="1101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1101" t="s">
         <v>1417</v>
       </c>
     </row>
-    <row r="1102" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1102" t="s">
         <v>4340</v>
       </c>
     </row>
-    <row r="1103" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1103" t="s">
         <v>1222</v>
       </c>
     </row>
-    <row r="1104" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1104" t="s">
         <v>1107</v>
       </c>
@@ -67486,140 +67852,263 @@
         <v>18</v>
       </c>
     </row>
-    <row r="1153" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1153" t="s">
         <v>527</v>
       </c>
     </row>
-    <row r="1154" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1154" t="s">
         <v>1630</v>
       </c>
     </row>
-    <row r="1155" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1155" t="s">
         <v>4363</v>
       </c>
     </row>
-    <row r="1156" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1156" t="s">
         <v>4364</v>
       </c>
     </row>
-    <row r="1157" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1157" t="s">
         <v>4556</v>
       </c>
     </row>
-    <row r="1158" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1158" t="s">
         <v>1104</v>
       </c>
     </row>
-    <row r="1159" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1159" t="s">
         <v>4365</v>
       </c>
     </row>
-    <row r="1160" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1160" t="s">
         <v>1299</v>
       </c>
     </row>
-    <row r="1161" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1161" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1161" t="s">
         <v>4366</v>
       </c>
     </row>
-    <row r="1162" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1162" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1162" t="s">
         <v>4367</v>
       </c>
     </row>
-    <row r="1163" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1163" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1163" t="s">
         <v>581</v>
       </c>
-    </row>
-    <row r="1164" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C1163">
+        <v>62</v>
+      </c>
+      <c r="D1163" t="s">
+        <v>4598</v>
+      </c>
+    </row>
+    <row r="1164" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1164" t="s">
         <v>810</v>
       </c>
     </row>
-    <row r="1165" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1165" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1165" t="s">
         <v>4368</v>
       </c>
     </row>
-    <row r="1166" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1166" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1166" t="s">
         <v>4369</v>
       </c>
     </row>
-    <row r="1167" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1167" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1167" t="s">
         <v>4370</v>
       </c>
-    </row>
-    <row r="1168" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B1167" t="s">
+        <v>4370</v>
+      </c>
+      <c r="C1167" t="s">
+        <v>4596</v>
+      </c>
+      <c r="D1167" t="s">
+        <v>4597</v>
+      </c>
+    </row>
+    <row r="1168" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1168" t="s">
         <v>4371</v>
+      </c>
+      <c r="B1168" t="s">
+        <v>4370</v>
+      </c>
+      <c r="C1168" t="s">
+        <v>4596</v>
+      </c>
+      <c r="D1168" t="s">
+        <v>4597</v>
       </c>
     </row>
     <row r="1169" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1169" t="s">
         <v>4557</v>
       </c>
+      <c r="B1169" t="s">
+        <v>4370</v>
+      </c>
+      <c r="C1169" t="s">
+        <v>4596</v>
+      </c>
+      <c r="D1169" t="s">
+        <v>4597</v>
+      </c>
     </row>
     <row r="1170" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1170" t="s">
         <v>29</v>
       </c>
+      <c r="B1170" t="s">
+        <v>4370</v>
+      </c>
+      <c r="C1170" t="s">
+        <v>4596</v>
+      </c>
+      <c r="D1170" t="s">
+        <v>4597</v>
+      </c>
     </row>
     <row r="1171" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1171" t="s">
         <v>835</v>
       </c>
+      <c r="B1171" t="s">
+        <v>4370</v>
+      </c>
+      <c r="C1171" t="s">
+        <v>4596</v>
+      </c>
+      <c r="D1171" t="s">
+        <v>4597</v>
+      </c>
     </row>
     <row r="1172" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1172" t="s">
         <v>4372</v>
       </c>
+      <c r="B1172" t="s">
+        <v>4370</v>
+      </c>
+      <c r="C1172" t="s">
+        <v>4596</v>
+      </c>
+      <c r="D1172" t="s">
+        <v>4597</v>
+      </c>
     </row>
     <row r="1173" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1173" t="s">
         <v>4373</v>
       </c>
+      <c r="B1173" t="s">
+        <v>4370</v>
+      </c>
+      <c r="C1173" t="s">
+        <v>4596</v>
+      </c>
+      <c r="D1173" t="s">
+        <v>4597</v>
+      </c>
     </row>
     <row r="1174" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1174" t="s">
         <v>4374</v>
       </c>
+      <c r="B1174" t="s">
+        <v>4370</v>
+      </c>
+      <c r="C1174" t="s">
+        <v>4596</v>
+      </c>
+      <c r="D1174" t="s">
+        <v>4597</v>
+      </c>
     </row>
     <row r="1175" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1175" t="s">
         <v>4375</v>
       </c>
+      <c r="B1175" t="s">
+        <v>4370</v>
+      </c>
+      <c r="C1175" t="s">
+        <v>4596</v>
+      </c>
+      <c r="D1175" t="s">
+        <v>4597</v>
+      </c>
     </row>
     <row r="1176" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1176" t="s">
         <v>4376</v>
       </c>
+      <c r="B1176" t="s">
+        <v>4370</v>
+      </c>
+      <c r="C1176" t="s">
+        <v>4596</v>
+      </c>
+      <c r="D1176" t="s">
+        <v>4597</v>
+      </c>
     </row>
     <row r="1177" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1177" t="s">
         <v>4377</v>
       </c>
+      <c r="B1177" t="s">
+        <v>4370</v>
+      </c>
+      <c r="C1177" t="s">
+        <v>4596</v>
+      </c>
+      <c r="D1177" t="s">
+        <v>4597</v>
+      </c>
     </row>
     <row r="1178" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1178" t="s">
         <v>4378</v>
       </c>
+      <c r="B1178" t="s">
+        <v>4370</v>
+      </c>
+      <c r="C1178" t="s">
+        <v>4596</v>
+      </c>
+      <c r="D1178" t="s">
+        <v>4597</v>
+      </c>
     </row>
     <row r="1179" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1179" t="s">
         <v>1260</v>
       </c>
+      <c r="B1179" t="s">
+        <v>4370</v>
+      </c>
+      <c r="C1179" t="s">
+        <v>4596</v>
+      </c>
+      <c r="D1179" t="s">
+        <v>4597</v>
+      </c>
     </row>
     <row r="1180" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1180" t="s">
@@ -67655,242 +68144,380 @@
         <v>3303</v>
       </c>
     </row>
-    <row r="1185" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1185" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1185" t="s">
         <v>3604</v>
       </c>
     </row>
-    <row r="1186" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1186" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1186" t="s">
         <v>4381</v>
       </c>
     </row>
-    <row r="1187" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1187" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1187" t="s">
         <v>4382</v>
       </c>
     </row>
-    <row r="1188" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1188" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1188" t="s">
         <v>4383</v>
       </c>
     </row>
-    <row r="1189" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1189" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1189" t="s">
         <v>1118</v>
       </c>
     </row>
-    <row r="1190" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1190" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1190" t="s">
         <v>4384</v>
       </c>
     </row>
-    <row r="1191" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1191" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1191" t="s">
         <v>1382</v>
       </c>
     </row>
-    <row r="1192" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1192" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1192" t="s">
         <v>1014</v>
       </c>
     </row>
-    <row r="1193" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1193" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1193" t="s">
         <v>1342</v>
       </c>
     </row>
-    <row r="1194" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1194" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1194" t="s">
         <v>4385</v>
       </c>
     </row>
-    <row r="1195" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1195" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1195" t="s">
         <v>4386</v>
       </c>
     </row>
-    <row r="1196" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1196" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1196" t="s">
         <v>3547</v>
       </c>
     </row>
-    <row r="1197" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1197" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1197" t="s">
         <v>1294</v>
       </c>
     </row>
-    <row r="1198" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1198" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1198" t="s">
         <v>1604</v>
       </c>
-    </row>
-    <row r="1199" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C1198">
+        <v>62</v>
+      </c>
+      <c r="D1198" t="s">
+        <v>4598</v>
+      </c>
+    </row>
+    <row r="1199" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1199" t="s">
         <v>4387</v>
       </c>
     </row>
-    <row r="1200" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1200" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1200" t="s">
         <v>1303</v>
       </c>
     </row>
-    <row r="1201" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1201" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1201" t="s">
         <v>1330</v>
       </c>
-    </row>
-    <row r="1202" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B1201" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C1201">
+        <v>72</v>
+      </c>
+      <c r="D1201" t="s">
+        <v>4601</v>
+      </c>
+    </row>
+    <row r="1202" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1202" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="1203" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B1202" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C1202">
+        <v>72</v>
+      </c>
+      <c r="D1202" t="s">
+        <v>4601</v>
+      </c>
+    </row>
+    <row r="1203" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1203" t="s">
         <v>4388</v>
       </c>
-    </row>
-    <row r="1204" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B1203" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C1203">
+        <v>72</v>
+      </c>
+      <c r="D1203" t="s">
+        <v>4601</v>
+      </c>
+    </row>
+    <row r="1204" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1204" t="s">
         <v>3425</v>
       </c>
-    </row>
-    <row r="1205" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B1204" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C1204">
+        <v>72</v>
+      </c>
+      <c r="D1204" t="s">
+        <v>4601</v>
+      </c>
+    </row>
+    <row r="1205" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1205" t="s">
         <v>3451</v>
       </c>
-    </row>
-    <row r="1206" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B1205" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C1205">
+        <v>72</v>
+      </c>
+      <c r="D1205" t="s">
+        <v>4601</v>
+      </c>
+    </row>
+    <row r="1206" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1206" t="s">
         <v>1096</v>
       </c>
-    </row>
-    <row r="1207" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B1206" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C1206">
+        <v>72</v>
+      </c>
+      <c r="D1206" t="s">
+        <v>4601</v>
+      </c>
+    </row>
+    <row r="1207" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1207" t="s">
         <v>857</v>
       </c>
-    </row>
-    <row r="1208" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B1207" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C1207">
+        <v>72</v>
+      </c>
+      <c r="D1207" t="s">
+        <v>4601</v>
+      </c>
+    </row>
+    <row r="1208" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1208" t="s">
         <v>3415</v>
       </c>
-    </row>
-    <row r="1209" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B1208" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C1208">
+        <v>72</v>
+      </c>
+      <c r="D1208" t="s">
+        <v>4601</v>
+      </c>
+    </row>
+    <row r="1209" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1209" t="s">
         <v>602</v>
       </c>
-    </row>
-    <row r="1210" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B1209" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C1209">
+        <v>72</v>
+      </c>
+      <c r="D1209" t="s">
+        <v>4601</v>
+      </c>
+    </row>
+    <row r="1210" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1210" t="s">
         <v>1065</v>
       </c>
-    </row>
-    <row r="1211" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B1210" t="s">
+        <v>4602</v>
+      </c>
+      <c r="C1210" t="s">
+        <v>4596</v>
+      </c>
+      <c r="D1210" t="s">
+        <v>4597</v>
+      </c>
+    </row>
+    <row r="1211" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1211" t="s">
         <v>1286</v>
       </c>
     </row>
-    <row r="1212" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1212" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1212" t="s">
         <v>4389</v>
       </c>
     </row>
-    <row r="1213" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1213" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1213" t="s">
         <v>4390</v>
       </c>
-    </row>
-    <row r="1214" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C1213">
+        <v>71</v>
+      </c>
+      <c r="D1213" t="s">
+        <v>4574</v>
+      </c>
+    </row>
+    <row r="1214" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1214" t="s">
         <v>4391</v>
       </c>
-    </row>
-    <row r="1215" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C1214">
+        <v>71</v>
+      </c>
+      <c r="D1214" t="s">
+        <v>4574</v>
+      </c>
+    </row>
+    <row r="1215" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1215" t="s">
         <v>4392</v>
       </c>
     </row>
-    <row r="1216" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1216" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1216" t="s">
         <v>1141</v>
       </c>
-    </row>
-    <row r="1217" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C1216">
+        <v>62</v>
+      </c>
+      <c r="D1216" t="s">
+        <v>4598</v>
+      </c>
+    </row>
+    <row r="1217" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1217" t="s">
         <v>1380</v>
       </c>
-    </row>
-    <row r="1218" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C1217">
+        <v>62</v>
+      </c>
+      <c r="D1217" t="s">
+        <v>4598</v>
+      </c>
+    </row>
+    <row r="1218" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1218" t="s">
         <v>3481</v>
       </c>
-    </row>
-    <row r="1219" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C1218">
+        <v>62</v>
+      </c>
+      <c r="D1218" t="s">
+        <v>4598</v>
+      </c>
+    </row>
+    <row r="1219" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1219" t="s">
         <v>4393</v>
       </c>
-    </row>
-    <row r="1220" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C1219">
+        <v>62</v>
+      </c>
+      <c r="D1219" t="s">
+        <v>4598</v>
+      </c>
+    </row>
+    <row r="1220" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1220" t="s">
         <v>1193</v>
       </c>
     </row>
-    <row r="1221" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1221" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1221" t="s">
         <v>1267</v>
       </c>
     </row>
-    <row r="1222" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1222" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1222" t="s">
         <v>533</v>
       </c>
     </row>
-    <row r="1223" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1223" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1223" t="s">
         <v>3561</v>
       </c>
     </row>
-    <row r="1224" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1224" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1224" t="s">
         <v>4394</v>
       </c>
     </row>
-    <row r="1225" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1225" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1225" t="s">
         <v>4395</v>
       </c>
     </row>
-    <row r="1226" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1226" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1226" t="s">
         <v>4396</v>
       </c>
     </row>
-    <row r="1227" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1227" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1227" t="s">
         <v>4397</v>
       </c>
     </row>
-    <row r="1228" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1228" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1228" t="s">
         <v>3444</v>
       </c>
-    </row>
-    <row r="1229" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C1228">
+        <v>62</v>
+      </c>
+      <c r="D1228" t="s">
+        <v>4598</v>
+      </c>
+    </row>
+    <row r="1229" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1229" t="s">
         <v>1638</v>
       </c>
     </row>
-    <row r="1230" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1230" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1230" t="s">
         <v>4398</v>
       </c>
     </row>
-    <row r="1231" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1231" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1231" t="s">
         <v>1434</v>
       </c>
     </row>
-    <row r="1232" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1232" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1232" t="s">
         <v>1373</v>
       </c>
@@ -68133,11 +68760,23 @@
       <c r="A1278" t="s">
         <v>4417</v>
       </c>
+      <c r="C1278">
+        <v>52</v>
+      </c>
+      <c r="D1278" t="s">
+        <v>4568</v>
+      </c>
     </row>
     <row r="1279" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1279" t="s">
         <v>3564</v>
       </c>
+      <c r="C1279">
+        <v>72</v>
+      </c>
+      <c r="D1279" t="s">
+        <v>4601</v>
+      </c>
     </row>
     <row r="1280" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1280" t="s">
@@ -68281,164 +68920,254 @@
         <v>4423</v>
       </c>
     </row>
-    <row r="1297" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1297" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1297" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="1298" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1298" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1298" t="s">
         <v>1180</v>
       </c>
     </row>
-    <row r="1299" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1299" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1299" t="s">
         <v>4424</v>
       </c>
-    </row>
-    <row r="1300" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C1299" t="s">
+        <v>4569</v>
+      </c>
+      <c r="D1299" t="s">
+        <v>4570</v>
+      </c>
+    </row>
+    <row r="1300" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1300" t="s">
         <v>4425</v>
       </c>
     </row>
-    <row r="1301" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1301" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1301" t="s">
         <v>1410</v>
       </c>
     </row>
-    <row r="1302" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1302" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1302" t="s">
         <v>4426</v>
       </c>
     </row>
-    <row r="1303" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1303" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1303" t="s">
         <v>1258</v>
       </c>
     </row>
-    <row r="1304" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1304" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1304" t="s">
         <v>1374</v>
       </c>
     </row>
-    <row r="1305" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1305" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1305" t="s">
         <v>1337</v>
       </c>
     </row>
-    <row r="1306" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1306" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1306" t="s">
         <v>4427</v>
       </c>
     </row>
-    <row r="1307" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1307" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1307" t="s">
         <v>4428</v>
       </c>
     </row>
-    <row r="1308" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1308" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1308" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="1309" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1309" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1309" t="s">
         <v>4558</v>
       </c>
-    </row>
-    <row r="1310" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C1309">
+        <v>71</v>
+      </c>
+      <c r="D1309" t="s">
+        <v>4574</v>
+      </c>
+    </row>
+    <row r="1310" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1310" t="s">
         <v>4429</v>
       </c>
     </row>
-    <row r="1311" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1311" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1311" t="s">
         <v>4430</v>
       </c>
     </row>
-    <row r="1312" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1312" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1312" t="s">
         <v>4431</v>
       </c>
     </row>
-    <row r="1313" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1313" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1313" t="s">
         <v>1058</v>
       </c>
     </row>
-    <row r="1314" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1314" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1314" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="1315" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1315" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1315" t="s">
         <v>4559</v>
       </c>
-    </row>
-    <row r="1316" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C1315" t="s">
+        <v>4596</v>
+      </c>
+      <c r="D1315" t="s">
+        <v>4597</v>
+      </c>
+    </row>
+    <row r="1316" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1316" t="s">
         <v>840</v>
       </c>
     </row>
-    <row r="1317" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1317" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1317" t="s">
         <v>4432</v>
       </c>
-    </row>
-    <row r="1318" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B1317" t="s">
+        <v>4433</v>
+      </c>
+      <c r="C1317">
+        <v>51</v>
+      </c>
+      <c r="D1317" t="s">
+        <v>4600</v>
+      </c>
+    </row>
+    <row r="1318" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1318" t="s">
         <v>4433</v>
       </c>
-    </row>
-    <row r="1319" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B1318" t="s">
+        <v>4433</v>
+      </c>
+      <c r="C1318">
+        <v>51</v>
+      </c>
+      <c r="D1318" t="s">
+        <v>4600</v>
+      </c>
+    </row>
+    <row r="1319" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1319" t="s">
         <v>4434</v>
       </c>
-    </row>
-    <row r="1320" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B1319" t="s">
+        <v>4433</v>
+      </c>
+      <c r="C1319">
+        <v>51</v>
+      </c>
+      <c r="D1319" t="s">
+        <v>4600</v>
+      </c>
+    </row>
+    <row r="1320" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1320" t="s">
         <v>4435</v>
       </c>
-    </row>
-    <row r="1321" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B1320" t="s">
+        <v>4433</v>
+      </c>
+      <c r="C1320">
+        <v>51</v>
+      </c>
+      <c r="D1320" t="s">
+        <v>4600</v>
+      </c>
+    </row>
+    <row r="1321" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1321" t="s">
         <v>4436</v>
       </c>
-    </row>
-    <row r="1322" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B1321" t="s">
+        <v>4433</v>
+      </c>
+      <c r="C1321">
+        <v>51</v>
+      </c>
+      <c r="D1321" t="s">
+        <v>4600</v>
+      </c>
+    </row>
+    <row r="1322" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1322" t="s">
         <v>4437</v>
       </c>
-    </row>
-    <row r="1323" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B1322" t="s">
+        <v>4433</v>
+      </c>
+      <c r="C1322">
+        <v>51</v>
+      </c>
+      <c r="D1322" t="s">
+        <v>4600</v>
+      </c>
+    </row>
+    <row r="1323" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1323" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="1324" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1324" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1324" t="s">
         <v>1270</v>
       </c>
     </row>
-    <row r="1325" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1325" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1325" t="s">
         <v>3226</v>
       </c>
     </row>
-    <row r="1326" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1326" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1326" t="s">
         <v>417</v>
       </c>
-    </row>
-    <row r="1327" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C1326">
+        <v>71</v>
+      </c>
+      <c r="D1326" t="s">
+        <v>4574</v>
+      </c>
+    </row>
+    <row r="1327" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1327" t="s">
         <v>429</v>
       </c>
-    </row>
-    <row r="1328" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C1327">
+        <v>71</v>
+      </c>
+      <c r="D1327" t="s">
+        <v>4574</v>
+      </c>
+    </row>
+    <row r="1328" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1328" t="s">
         <v>446</v>
+      </c>
+      <c r="C1328" t="s">
+        <v>4569</v>
+      </c>
+      <c r="D1328" t="s">
+        <v>4570</v>
       </c>
     </row>
     <row r="1329" spans="1:4" x14ac:dyDescent="0.2">
@@ -68455,11 +69184,29 @@
       <c r="A1331" t="s">
         <v>4438</v>
       </c>
+      <c r="B1331" t="s">
+        <v>4438</v>
+      </c>
+      <c r="C1331" t="s">
+        <v>4569</v>
+      </c>
+      <c r="D1331" t="s">
+        <v>4570</v>
+      </c>
     </row>
     <row r="1332" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1332" t="s">
         <v>4439</v>
       </c>
+      <c r="B1332" t="s">
+        <v>4438</v>
+      </c>
+      <c r="C1332" t="s">
+        <v>4569</v>
+      </c>
+      <c r="D1332" t="s">
+        <v>4570</v>
+      </c>
     </row>
     <row r="1333" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1333" t="s">
@@ -68690,82 +69437,88 @@
         <v>4459</v>
       </c>
     </row>
-    <row r="1377" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1377" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1377" t="s">
         <v>1354</v>
       </c>
     </row>
-    <row r="1378" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1378" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1378" t="s">
         <v>1292</v>
       </c>
     </row>
-    <row r="1379" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1379" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1379" t="s">
         <v>4460</v>
       </c>
     </row>
-    <row r="1380" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1380" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1380" t="s">
         <v>4461</v>
       </c>
     </row>
-    <row r="1381" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1381" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1381" t="s">
         <v>4462</v>
       </c>
     </row>
-    <row r="1382" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1382" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1382" t="s">
         <v>587</v>
       </c>
     </row>
-    <row r="1383" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1383" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1383" t="s">
         <v>1291</v>
       </c>
     </row>
-    <row r="1384" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1384" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1384" t="s">
         <v>4463</v>
       </c>
     </row>
-    <row r="1385" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1385" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1385" t="s">
         <v>4464</v>
       </c>
     </row>
-    <row r="1386" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1386" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1386" t="s">
         <v>4465</v>
       </c>
     </row>
-    <row r="1387" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1387" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1387" t="s">
         <v>1457</v>
       </c>
     </row>
-    <row r="1388" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1388" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1388" t="s">
         <v>4466</v>
       </c>
-    </row>
-    <row r="1389" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C1388">
+        <v>71</v>
+      </c>
+      <c r="D1388" t="s">
+        <v>4574</v>
+      </c>
+    </row>
+    <row r="1389" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1389" t="s">
         <v>1249</v>
       </c>
     </row>
-    <row r="1390" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1390" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1390" t="s">
         <v>1300</v>
       </c>
     </row>
-    <row r="1391" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1391" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1391" t="s">
         <v>994</v>
       </c>
     </row>
-    <row r="1392" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1392" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1392" t="s">
         <v>4467</v>
       </c>
@@ -69324,6 +70077,12 @@
       <c r="A1455" t="s">
         <v>4488</v>
       </c>
+      <c r="C1455" t="s">
+        <v>4569</v>
+      </c>
+      <c r="D1455" t="s">
+        <v>4570</v>
+      </c>
     </row>
     <row r="1456" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1456" t="s">
@@ -69371,11 +70130,23 @@
       <c r="A1462" t="s">
         <v>4491</v>
       </c>
+      <c r="C1462">
+        <v>56</v>
+      </c>
+      <c r="D1462" t="s">
+        <v>4599</v>
+      </c>
     </row>
     <row r="1463" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1463" t="s">
         <v>933</v>
       </c>
+      <c r="C1463">
+        <v>56</v>
+      </c>
+      <c r="D1463" t="s">
+        <v>4599</v>
+      </c>
     </row>
     <row r="1464" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1464" t="s">
@@ -69396,6 +70167,12 @@
       <c r="A1467" t="s">
         <v>4495</v>
       </c>
+      <c r="C1467">
+        <v>62</v>
+      </c>
+      <c r="D1467" t="s">
+        <v>4598</v>
+      </c>
     </row>
     <row r="1468" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1468" t="s">
@@ -69406,6 +70183,12 @@
       <c r="A1469" t="s">
         <v>3274</v>
       </c>
+      <c r="C1469">
+        <v>71</v>
+      </c>
+      <c r="D1469" t="s">
+        <v>4574</v>
+      </c>
     </row>
     <row r="1470" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1470" t="s">
@@ -69466,6 +70249,12 @@
       <c r="A1481" t="s">
         <v>1389</v>
       </c>
+      <c r="C1481">
+        <v>62</v>
+      </c>
+      <c r="D1481" t="s">
+        <v>4598</v>
+      </c>
     </row>
     <row r="1482" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1482" t="s">
@@ -69609,82 +70398,142 @@
         <v>4512</v>
       </c>
     </row>
-    <row r="1505" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1505" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1505" t="s">
         <v>3421</v>
       </c>
     </row>
-    <row r="1506" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1506" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1506" t="s">
         <v>996</v>
       </c>
-    </row>
-    <row r="1507" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C1506" t="s">
+        <v>4594</v>
+      </c>
+      <c r="D1506" t="s">
+        <v>4595</v>
+      </c>
+    </row>
+    <row r="1507" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1507" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="1508" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C1507" t="s">
+        <v>4594</v>
+      </c>
+      <c r="D1507" t="s">
+        <v>4595</v>
+      </c>
+    </row>
+    <row r="1508" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1508" t="s">
         <v>1077</v>
       </c>
-    </row>
-    <row r="1509" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C1508" t="s">
+        <v>4594</v>
+      </c>
+      <c r="D1508" t="s">
+        <v>4595</v>
+      </c>
+    </row>
+    <row r="1509" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1509" t="s">
         <v>3534</v>
       </c>
     </row>
-    <row r="1510" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1510" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1510" t="s">
         <v>4513</v>
       </c>
-    </row>
-    <row r="1511" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C1510" t="s">
+        <v>4596</v>
+      </c>
+      <c r="D1510" t="s">
+        <v>4597</v>
+      </c>
+    </row>
+    <row r="1511" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1511" t="s">
         <v>4562</v>
       </c>
     </row>
-    <row r="1512" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1512" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1512" t="s">
         <v>844</v>
       </c>
     </row>
-    <row r="1513" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1513" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1513" t="s">
         <v>937</v>
       </c>
     </row>
-    <row r="1514" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1514" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1514" t="s">
         <v>613</v>
       </c>
     </row>
-    <row r="1515" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1515" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1515" t="s">
         <v>3382</v>
       </c>
-    </row>
-    <row r="1516" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B1515" t="s">
+        <v>4593</v>
+      </c>
+      <c r="C1515">
+        <v>71</v>
+      </c>
+      <c r="D1515" t="s">
+        <v>4574</v>
+      </c>
+    </row>
+    <row r="1516" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1516" t="s">
         <v>3380</v>
       </c>
-    </row>
-    <row r="1517" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B1516" t="s">
+        <v>4593</v>
+      </c>
+      <c r="C1516">
+        <v>71</v>
+      </c>
+      <c r="D1516" t="s">
+        <v>4574</v>
+      </c>
+    </row>
+    <row r="1517" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1517" t="s">
         <v>3386</v>
       </c>
-    </row>
-    <row r="1518" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B1517" t="s">
+        <v>4593</v>
+      </c>
+      <c r="C1517">
+        <v>71</v>
+      </c>
+      <c r="D1517" t="s">
+        <v>4574</v>
+      </c>
+    </row>
+    <row r="1518" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1518" t="s">
         <v>3384</v>
       </c>
-    </row>
-    <row r="1519" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B1518" t="s">
+        <v>4593</v>
+      </c>
+      <c r="C1518">
+        <v>71</v>
+      </c>
+      <c r="D1518" t="s">
+        <v>4574</v>
+      </c>
+    </row>
+    <row r="1519" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1519" t="s">
         <v>4563</v>
       </c>
     </row>
-    <row r="1520" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1520" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1520" t="s">
         <v>1142</v>
       </c>

</xml_diff>